<commit_message>
Segment 3 Deliverable due 6/21/20
</commit_message>
<xml_diff>
--- a/Resources/Random Forest Analysis-final.xlsx
+++ b/Resources/Random Forest Analysis-final.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="154" documentId="8_{B2E74B40-5D98-41C8-BCDD-914FA1A8BB00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{3D77DC2E-0DE6-49B9-97A4-4DD1D0A11172}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A4224A1-CC55-4A8E-8132-71ABCE4FE425}"/>
+    <workbookView xWindow="24864" yWindow="1824" windowWidth="17280" windowHeight="8916" xr2:uid="{8A4224A1-CC55-4A8E-8132-71ABCE4FE425}"/>
   </bookViews>
   <sheets>
     <sheet name="Classification Metrics" sheetId="3" r:id="rId1"/>
@@ -413,16 +413,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21D34D5-1A7B-4765-BEDF-18BADC340302}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -751,12 +751,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
@@ -833,14 +833,14 @@
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
@@ -863,16 +863,16 @@
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="17">
         <v>0.72</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="17">
         <v>0.47</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="17">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="18">
         <v>136</v>
       </c>
     </row>
@@ -880,36 +880,36 @@
       <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="17">
         <v>0.67</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="17">
         <v>0.86</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="17">
         <v>0.75</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="18">
         <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17">
         <v>0.69</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="18">
         <v>310</v>
       </c>
     </row>
@@ -917,16 +917,16 @@
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="17">
         <v>0.7</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="17">
         <v>0.66</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="17">
         <v>0.67</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="18">
         <v>310</v>
       </c>
     </row>
@@ -934,24 +934,24 @@
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="17">
         <v>0.69</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="17">
         <v>0.69</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="17">
         <v>0.68</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="18">
         <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="20"/>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
@@ -1467,6 +1467,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B03C3E295CF76648AC85B6EC26361ECA" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0bb9dd14d241c245318bb8942e244b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b42430d8-c205-408e-a6b2-f7bcf1ddda46" xmlns:ns4="076ed714-3a77-4f17-8bbf-04471c3fc2e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d56a7a2c73efd02ab063fa24f087166" ns3:_="" ns4:_="">
     <xsd:import namespace="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
@@ -1689,22 +1704,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0FB5970-FED5-40C8-AA2E-DA5923CD693C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDC7EADE-C10B-47E7-8CF9-C6F7975E8804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
+    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3C80D87-A783-4212-876E-82900FFF8A9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1721,29 +1746,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDC7EADE-C10B-47E7-8CF9-C6F7975E8804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0FB5970-FED5-40C8-AA2E-DA5923CD693C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>